<commit_message>
Update docs for 1.37.0
</commit_message>
<xml_diff>
--- a/StructureDefinition-additional-planned-travel-destination-country.xlsx
+++ b/StructureDefinition-additional-planned-travel-destination-country.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-09-07T08:24:04-04:00</t>
+    <t>2021-10-06T18:59:21-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Represents destination country of the monitoree’s planned travel. This field is read-only.</t>
+    <t>Represents destination country of the monitoree’s planned travel.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>